<commit_message>
Negociado de la Policia
INCIDENTES DE VIOLENCIA DOMÉSTICA POR ÁREA. ENERO - OCTUBRE 2023
</commit_message>
<xml_diff>
--- a/data/Negociado_de_Policia/Incidentes Violencia Domestica por area policiaca.xlsx
+++ b/data/Negociado_de_Policia/Incidentes Violencia Domestica por area policiaca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2f9f81cad9707229/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2f9f81cad9707229/Documents/GitHub/Estadisticas-Sobre-Violencia-de-Genero-en-Puerto-Rico/data/Negociado_de_Policia/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{B5D772A3-C86A-4736-BB47-FEF3B54E33FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>